<commit_message>
rename sheets in sample excel data files
</commit_message>
<xml_diff>
--- a/jasperreports/demo/samples/exceldataadapter/data/data.xlsx
+++ b/jasperreports/demo/samples/exceldataadapter/data/data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teodor/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392C0703-4598-A941-B0DA-3EAFEB0F363E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="XlsxDataSource1" sheetId="1" r:id="rId1"/>
-    <sheet name="XlsxDataSource2" sheetId="2" r:id="rId2"/>
-    <sheet name="XlsxDataSource3" sheetId="3" r:id="rId3"/>
+    <sheet name="Data Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Sheet 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Sheet 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
@@ -240,7 +246,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -285,6 +291,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -333,7 +342,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -366,9 +375,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -401,6 +427,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -576,24 +619,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125"/>
-    <col min="2" max="2" width="10.85546875"/>
-    <col min="3" max="3" width="20.140625"/>
-    <col min="4" max="4" width="23.85546875"/>
-    <col min="5" max="5" width="38.28515625"/>
-    <col min="6" max="6" width="28.28515625"/>
-    <col min="7" max="7" width="12.85546875"/>
-    <col min="8" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="24.5"/>
+    <col min="2" max="2" width="10.83203125"/>
+    <col min="3" max="3" width="20.1640625"/>
+    <col min="4" max="4" width="23.83203125"/>
+    <col min="5" max="5" width="38.33203125"/>
+    <col min="6" max="6" width="28.33203125"/>
+    <col min="7" max="7" width="12.83203125"/>
+    <col min="8" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +656,7 @@
         <v>40673</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -633,7 +676,7 @@
         <v>41375</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -653,7 +696,7 @@
         <v>40980</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -673,7 +716,7 @@
         <v>41407</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -693,7 +736,7 @@
         <v>40708</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -713,7 +756,7 @@
         <v>41470</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -733,7 +776,7 @@
         <v>41137</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -753,7 +796,7 @@
         <v>41564</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -773,7 +816,7 @@
         <v>40865</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -800,25 +843,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD65525"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.5703125"/>
-    <col min="3" max="3" width="19.42578125"/>
+    <col min="1" max="2" width="8.5"/>
+    <col min="3" max="3" width="19.5"/>
     <col min="4" max="4" width="27"/>
-    <col min="5" max="5" width="22.140625"/>
+    <col min="5" max="5" width="22.1640625"/>
     <col min="6" max="6" width="16"/>
-    <col min="7" max="7" width="11.140625"/>
-    <col min="8" max="1025" width="8.5703125"/>
+    <col min="7" max="7" width="11.1640625"/>
+    <col min="8" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -838,7 +881,7 @@
         <v>40673</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -858,7 +901,7 @@
         <v>41375</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -878,7 +921,7 @@
         <v>40980</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -898,7 +941,7 @@
         <v>41407</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -918,7 +961,7 @@
         <v>40708</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -938,7 +981,7 @@
         <v>41470</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -958,7 +1001,7 @@
         <v>41137</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -978,7 +1021,7 @@
         <v>41564</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -1005,26 +1048,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.140625"/>
-    <col min="2" max="2" width="8.5703125"/>
-    <col min="3" max="3" width="14.140625"/>
-    <col min="4" max="4" width="20.85546875"/>
-    <col min="5" max="5" width="23.28515625"/>
-    <col min="6" max="6" width="21.140625"/>
-    <col min="7" max="7" width="12.7109375"/>
-    <col min="8" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="20.1640625"/>
+    <col min="2" max="2" width="8.5"/>
+    <col min="3" max="3" width="14.1640625"/>
+    <col min="4" max="4" width="20.83203125"/>
+    <col min="5" max="5" width="23.33203125"/>
+    <col min="6" max="6" width="21.1640625"/>
+    <col min="7" max="7" width="12.6640625"/>
+    <col min="8" max="1025" width="8.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>46</v>
       </c>
@@ -1044,7 +1087,7 @@
         <v>40673</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1064,7 +1107,7 @@
         <v>41375</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1084,7 +1127,7 @@
         <v>40980</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1104,7 +1147,7 @@
         <v>41407</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -1124,7 +1167,7 @@
         <v>40708</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1144,7 +1187,7 @@
         <v>41470</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1164,7 +1207,7 @@
         <v>41137</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1184,7 +1227,7 @@
         <v>41564</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1204,7 +1247,7 @@
         <v>40865</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1224,7 +1267,7 @@
         <v>41627</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>59</v>
       </c>

</xml_diff>